<commit_message>
new high sequestration lulucf scenario
</commit_message>
<xml_diff>
--- a/data-extra/USDA NFS Raw Data/LULUCF projections DRAFT compilation 82924.xlsx
+++ b/data-extra/USDA NFS Raw Data/LULUCF projections DRAFT compilation 82924.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-extra\USDA NFS Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A750C1-880B-4AD9-B139-D8D31F5AB2F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65679AEC-7729-47B9-9AF2-D68498767309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="928" activeTab="1" xr2:uid="{5262EA9F-E3D4-48CB-897F-32B2FDC9F2FD}"/>
   </bookViews>
@@ -751,7 +751,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1083" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1088" uniqueCount="237">
   <si>
     <t>Table 6-2:  Emissions and Removals from Land Use, Land-Use Change, and Forestry by Gas (MMT CO2 Eq.)</t>
   </si>
@@ -31154,10 +31154,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B4A0C6-FB3D-48AD-8074-AF9061A88699}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31325,6 +31325,41 @@
       <c r="K4">
         <f>'LULUCF nonco2 all'!AA40</f>
         <v>9.4825687076057825</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5" t="s">
+        <v>231</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5" t="s">
+        <v>228</v>
+      </c>
+      <c r="E5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F5">
+        <v>-887.3</v>
+      </c>
+      <c r="G5">
+        <v>-942.745930000003</v>
+      </c>
+      <c r="H5">
+        <v>-1135.2007300000009</v>
+      </c>
+      <c r="I5">
+        <v>-1327.6555299999986</v>
+      </c>
+      <c r="J5">
+        <v>-1108.2721050000009</v>
+      </c>
+      <c r="K5">
+        <v>-888.88868000000298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to LULUCF forest only co2 data
</commit_message>
<xml_diff>
--- a/data-extra/USDA NFS Raw Data/LULUCF projections DRAFT compilation 82924.xlsx
+++ b/data-extra/USDA NFS Raw Data/LULUCF projections DRAFT compilation 82924.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-extra\USDA NFS Raw Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65679AEC-7729-47B9-9AF2-D68498767309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86824141-C41D-4426-9F57-744CB10365B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="928" activeTab="1" xr2:uid="{5262EA9F-E3D4-48CB-897F-32B2FDC9F2FD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="928" activeTab="7" xr2:uid="{5262EA9F-E3D4-48CB-897F-32B2FDC9F2FD}"/>
   </bookViews>
   <sheets>
     <sheet name="CTF Tbl 7" sheetId="15" r:id="rId1"/>
@@ -7311,7 +7311,7 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
+    <xxl21:alternateUrls driveId="b!NaNodoGU4Ui6vH60hPlJpSQWNNXfwUxGj4xnL_mAQnbt4soX-IoWQIMe1YhGH2MC" itemId="01VGIIB65BSJPOFD67RNCYOETOAYJF6ALI">
       <xxl21:absoluteUrl r:id="rId2"/>
     </xxl21:alternateUrls>
     <sheetNames>
@@ -11801,15 +11801,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:9" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="144.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="160" t="s">
         <v>165</v>
       </c>
@@ -11823,7 +11823,7 @@
       <c r="F2" s="167"/>
       <c r="G2" s="168"/>
     </row>
-    <row r="3" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="161" t="s">
         <v>168</v>
       </c>
@@ -11843,35 +11843,35 @@
         <v>2040</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="128" t="s">
         <v>169</v>
       </c>
       <c r="C4" s="129"/>
       <c r="G4" s="84"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="128" t="s">
         <v>170</v>
       </c>
       <c r="C5" s="129"/>
       <c r="G5" s="84"/>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="128" t="s">
         <v>171</v>
       </c>
       <c r="C6" s="129"/>
       <c r="G6" s="84"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="128" t="s">
         <v>172</v>
       </c>
       <c r="C7" s="129"/>
       <c r="G7" s="84"/>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="128" t="s">
         <v>173</v>
       </c>
@@ -11879,7 +11879,7 @@
       <c r="G8" s="84"/>
       <c r="I8" s="153"/>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="128" t="s">
         <v>174</v>
       </c>
@@ -11887,7 +11887,7 @@
       <c r="G9" s="84"/>
       <c r="I9" s="153"/>
     </row>
-    <row r="10" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="128" t="s">
         <v>175</v>
       </c>
@@ -11895,7 +11895,7 @@
       <c r="G10" s="84"/>
       <c r="I10" s="153"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="130" t="s">
         <v>176</v>
       </c>
@@ -11906,7 +11906,7 @@
       <c r="G11" s="132"/>
       <c r="I11" s="153"/>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="128" t="s">
         <v>177</v>
       </c>
@@ -11914,7 +11914,7 @@
       <c r="G12" s="84"/>
       <c r="I12" s="153"/>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="128" t="s">
         <v>178</v>
       </c>
@@ -11922,7 +11922,7 @@
       <c r="G13" s="84"/>
       <c r="I13" s="153"/>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="128" t="s">
         <v>179</v>
       </c>
@@ -11930,7 +11930,7 @@
       <c r="G14" s="84"/>
       <c r="I14" s="153"/>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="128" t="s">
         <v>180</v>
       </c>
@@ -11938,7 +11938,7 @@
       <c r="G15" s="84"/>
       <c r="I15" s="153"/>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="128" t="s">
         <v>181</v>
       </c>
@@ -11946,7 +11946,7 @@
       <c r="G16" s="84"/>
       <c r="I16" s="153"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="128" t="s">
         <v>182</v>
       </c>
@@ -11954,7 +11954,7 @@
       <c r="G17" s="84"/>
       <c r="I17" s="153"/>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="128" t="s">
         <v>183</v>
       </c>
@@ -11962,7 +11962,7 @@
       <c r="G18" s="84"/>
       <c r="I18" s="153"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="128" t="s">
         <v>184</v>
       </c>
@@ -11970,7 +11970,7 @@
       <c r="G19" s="84"/>
       <c r="I19" s="153"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="128" t="s">
         <v>185</v>
       </c>
@@ -11978,7 +11978,7 @@
       <c r="G20" s="84"/>
       <c r="I20" s="153"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="128" t="s">
         <v>186</v>
       </c>
@@ -11986,7 +11986,7 @@
       <c r="G21" s="84"/>
       <c r="I21" s="153"/>
     </row>
-    <row r="22" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="133" t="s">
         <v>175</v>
       </c>
@@ -11996,14 +11996,14 @@
       <c r="F22" s="90"/>
       <c r="G22" s="91"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="134" t="s">
         <v>187</v>
       </c>
       <c r="C23" s="129"/>
       <c r="G23" s="84"/>
     </row>
-    <row r="24" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="126" t="s">
         <v>188</v>
       </c>
@@ -12027,19 +12027,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="27">
         <v>45516</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2" s="25" t="s">
         <v>66</v>
       </c>
@@ -12058,7 +12058,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B3" s="23"/>
       <c r="C3" s="2" t="s">
         <v>65</v>
@@ -12074,7 +12074,7 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C4" s="2">
         <v>2005</v>
       </c>
@@ -12103,7 +12103,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -12138,7 +12138,7 @@
         <v>-31.7</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>6</v>
       </c>
@@ -12173,7 +12173,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -12208,7 +12208,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>8</v>
       </c>
@@ -12243,7 +12243,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>9</v>
       </c>
@@ -12278,7 +12278,7 @@
         <v>-10.6</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>10</v>
       </c>
@@ -12313,7 +12313,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>64</v>
       </c>
@@ -12348,7 +12348,7 @@
         <v>-134.80000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>12</v>
       </c>
@@ -12383,7 +12383,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="33" t="s">
         <v>67</v>
       </c>
@@ -12435,13 +12435,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -12449,7 +12449,7 @@
         <v>45530</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="140" t="s">
         <v>78</v>
       </c>
@@ -12457,7 +12457,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" s="141" t="s">
         <v>79</v>
       </c>
@@ -12648,7 +12648,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="141" t="s">
         <v>5</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" s="80" t="s">
         <v>82</v>
       </c>
@@ -13030,7 +13030,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="6" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="141" t="s">
         <v>6</v>
       </c>
@@ -13221,7 +13221,7 @@
         <v>30.662284616283618</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" s="80" t="s">
         <v>84</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>30.662284616283618</v>
       </c>
     </row>
-    <row r="8" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="141" t="s">
         <v>7</v>
       </c>
@@ -13603,7 +13603,7 @@
         <v>5.064333299052576</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" s="80" t="s">
         <v>82</v>
       </c>
@@ -13794,7 +13794,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" s="143" t="s">
         <v>86</v>
       </c>
@@ -13985,7 +13985,7 @@
         <v>0.59462816708368171</v>
       </c>
     </row>
-    <row r="11" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="141" t="s">
         <v>8</v>
       </c>
@@ -14176,7 +14176,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A12" s="80" t="s">
         <v>84</v>
       </c>
@@ -14367,7 +14367,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A13" s="141" t="s">
         <v>9</v>
       </c>
@@ -14558,7 +14558,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="14" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="80" t="s">
         <v>89</v>
       </c>
@@ -14749,7 +14749,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A15" s="21" t="s">
         <v>90</v>
       </c>
@@ -14940,7 +14940,7 @@
         <v>1.2737501172567186E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="80" t="s">
         <v>91</v>
       </c>
@@ -15131,7 +15131,7 @@
         <v>-11.1</v>
       </c>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
         <v>92</v>
       </c>
@@ -15322,7 +15322,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A18" s="31" t="s">
         <v>93</v>
       </c>
@@ -15513,7 +15513,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A19" s="21" t="s">
         <v>94</v>
       </c>
@@ -15704,7 +15704,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A20" s="141" t="s">
         <v>10</v>
       </c>
@@ -15895,7 +15895,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A21" s="80" t="s">
         <v>96</v>
       </c>
@@ -16086,7 +16086,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A22" s="142" t="s">
         <v>98</v>
       </c>
@@ -16277,7 +16277,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A23" s="80" t="s">
         <v>99</v>
       </c>
@@ -16468,7 +16468,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A24" s="142" t="s">
         <v>100</v>
       </c>
@@ -16659,7 +16659,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A25" s="141" t="s">
         <v>11</v>
       </c>
@@ -16850,7 +16850,7 @@
         <v>-168.54883875480226</v>
       </c>
     </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A26" s="80" t="s">
         <v>102</v>
       </c>
@@ -17041,7 +17041,7 @@
         <v>19.604623238851623</v>
       </c>
     </row>
-    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A27" s="80" t="s">
         <v>103</v>
       </c>
@@ -17232,7 +17232,7 @@
         <v>-176.31430640136037</v>
       </c>
     </row>
-    <row r="28" spans="1:63" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="144" t="s">
         <v>104</v>
       </c>
@@ -17423,7 +17423,7 @@
         <v>3.1825687076057827</v>
       </c>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A29" s="80" t="s">
         <v>105</v>
       </c>
@@ -17614,7 +17614,7 @@
         <v>-15.021724299899295</v>
       </c>
     </row>
-    <row r="30" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="141" t="s">
         <v>12</v>
       </c>
@@ -17805,7 +17805,7 @@
         <v>72.635614317085398</v>
       </c>
     </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A31" s="80" t="s">
         <v>84</v>
       </c>
@@ -17996,7 +17996,7 @@
         <v>72.635614317085398</v>
       </c>
     </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:63" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>199</v>
       </c>
@@ -18245,12 +18245,12 @@
         <v>-99.475333293592811</v>
       </c>
     </row>
-    <row r="34" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -18499,7 +18499,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="36" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A36" t="str">
         <f>A4</f>
         <v>Cropland Remaining Cropland</v>
@@ -18508,7 +18508,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A37" t="str">
         <f>A6</f>
         <v>Land Converted to Cropland</v>
@@ -18517,7 +18517,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A38" s="143" t="str">
         <f>A8</f>
         <v>Grassland Remaining Grassland</v>
@@ -18767,7 +18767,7 @@
         <v>0.59462816708368171</v>
       </c>
     </row>
-    <row r="39" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A39" t="str">
         <f>A11</f>
         <v>Land Converted to Grassland</v>
@@ -18776,7 +18776,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="21" t="str">
         <f>A13</f>
         <v>Wetlands Remaining Wetlands</v>
@@ -19026,7 +19026,7 @@
         <v>48.500127375011729</v>
       </c>
     </row>
-    <row r="41" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A41" s="142" t="str">
         <f>A20</f>
         <v>Land Converted to Wetlands</v>
@@ -19276,7 +19276,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A42" t="str">
         <f>A25</f>
         <v>Settlements Remaining Settlements</v>
@@ -19285,7 +19285,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A43" t="str">
         <f>A30</f>
         <v>Land Converted to Settlements</v>
@@ -19294,12 +19294,12 @@
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:63" x14ac:dyDescent="0.3">
       <c r="B44" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:63" x14ac:dyDescent="0.3">
       <c r="C45" s="2">
         <f>SUM(C36:C43)</f>
         <v>49.90023985513772</v>
@@ -19545,7 +19545,7 @@
         <v>49.494755542095412</v>
       </c>
     </row>
-    <row r="46" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:63" x14ac:dyDescent="0.3">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -19608,7 +19608,7 @@
       <c r="BJ46" s="2"/>
       <c r="BK46" s="2"/>
     </row>
-    <row r="47" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="48" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -19804,7 +19804,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -19812,7 +19812,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -19826,7 +19826,7 @@
       <c r="AP50" s="92"/>
       <c r="AQ50" s="92"/>
     </row>
-    <row r="51" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -19834,7 +19834,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -20083,7 +20083,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -20091,7 +20091,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -20340,7 +20340,7 @@
         <v>3.1825687076057827</v>
       </c>
     </row>
-    <row r="55" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -20348,15 +20348,15 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="58" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="2">
         <f>SUM(C48:C55)</f>
         <v>2.2000000000000002</v>
@@ -20602,7 +20602,7 @@
         <v>3.2825687076057828</v>
       </c>
     </row>
-    <row r="64" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AL64" s="2" t="s">
         <v>121</v>
       </c>
@@ -20610,7 +20610,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>121</v>
       </c>
@@ -20798,7 +20798,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="66" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>5</v>
       </c>
@@ -21047,7 +21047,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="67" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>6</v>
       </c>
@@ -21296,7 +21296,7 @@
         <v>30.662284616283618</v>
       </c>
     </row>
-    <row r="68" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>7</v>
       </c>
@@ -21545,7 +21545,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="69" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>8</v>
       </c>
@@ -21794,7 +21794,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="70" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A70" s="80" t="s">
         <v>9</v>
       </c>
@@ -22043,7 +22043,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="71" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>10</v>
       </c>
@@ -22292,7 +22292,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="72" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>11</v>
       </c>
@@ -22541,7 +22541,7 @@
         <v>-171.73140746240804</v>
       </c>
     </row>
-    <row r="73" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>12</v>
       </c>
@@ -22790,12 +22790,12 @@
         <v>72.635614317085398</v>
       </c>
     </row>
-    <row r="74" spans="1:63" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:63" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="75" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C75" s="2">
         <f>SUM(C66:C73)</f>
         <v>40.499999999999993</v>
@@ -23041,7 +23041,7 @@
         <v>-99.475333293592811</v>
       </c>
     </row>
-    <row r="80" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AL80">
         <v>2025</v>
       </c>
@@ -23061,7 +23061,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="81" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="81" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL81">
         <v>-64.598787754204238</v>
       </c>
@@ -23081,7 +23081,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="82" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="82" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL82">
         <v>31.7107510794714</v>
       </c>
@@ -23101,7 +23101,7 @@
         <v>30.662284616283618</v>
       </c>
     </row>
-    <row r="83" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="83" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL83">
         <v>2.3996110699831004</v>
       </c>
@@ -23121,7 +23121,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="84" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="84" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL84">
         <v>25.557913188427918</v>
       </c>
@@ -23141,7 +23141,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="85" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="85" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL85">
         <v>-10.5</v>
       </c>
@@ -23161,7 +23161,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="86" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="86" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL86">
         <v>0.3</v>
       </c>
@@ -23181,7 +23181,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="87" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="87" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL87">
         <v>-138.62441009605425</v>
       </c>
@@ -23201,7 +23201,7 @@
         <v>-171.73140746240804</v>
       </c>
     </row>
-    <row r="88" spans="38:43" x14ac:dyDescent="0.25">
+    <row r="88" spans="38:43" x14ac:dyDescent="0.3">
       <c r="AL88">
         <v>58.632659776427879</v>
       </c>
@@ -23233,12 +23233,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>62</v>
       </c>
@@ -23250,7 +23250,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -23265,7 +23265,7 @@
       </c>
       <c r="AN2" s="3"/>
     </row>
-    <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -23387,7 +23387,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -23509,7 +23509,7 @@
         <v>-597.80079573463001</v>
       </c>
     </row>
-    <row r="5" spans="1:40" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>56</v>
       </c>
@@ -23664,7 +23664,7 @@
         <v>-474.77478093796299</v>
       </c>
     </row>
-    <row r="6" spans="1:40" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="18" t="s">
         <v>57</v>
       </c>
@@ -23819,7 +23819,7 @@
         <v>-123.026014796667</v>
       </c>
     </row>
-    <row r="7" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -23941,7 +23941,7 @@
         <v>-82.704318361679299</v>
       </c>
     </row>
-    <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>58</v>
       </c>
@@ -24102,7 +24102,7 @@
         <v>-680.50511409630928</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI9" s="11"/>
       <c r="AJ9" s="2"/>
       <c r="AK9" s="2"/>
@@ -24110,7 +24110,7 @@
       <c r="AM9" s="2"/>
       <c r="AN9" s="12"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI10" s="11"/>
       <c r="AJ10" s="2"/>
       <c r="AK10" s="2"/>
@@ -24118,7 +24118,7 @@
       <c r="AM10" s="2"/>
       <c r="AN10" s="12"/>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -24129,7 +24129,7 @@
       <c r="AM11" s="2"/>
       <c r="AN11" s="12"/>
     </row>
-    <row r="12" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -24239,7 +24239,7 @@
       <c r="AM12" s="9"/>
       <c r="AN12" s="10"/>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -24349,7 +24349,7 @@
       <c r="AM13" s="2"/>
       <c r="AN13" s="12"/>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -24459,7 +24459,7 @@
       <c r="AM14" s="2"/>
       <c r="AN14" s="12"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI15" s="11"/>
       <c r="AJ15" s="2"/>
       <c r="AK15" s="2"/>
@@ -24467,7 +24467,7 @@
       <c r="AM15" s="2"/>
       <c r="AN15" s="12"/>
     </row>
-    <row r="16" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>19</v>
       </c>
@@ -24577,7 +24577,7 @@
       <c r="AM16" s="9"/>
       <c r="AN16" s="10"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -24687,7 +24687,7 @@
       <c r="AM17" s="2"/>
       <c r="AN17" s="12"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -24797,7 +24797,7 @@
       <c r="AM18" s="2"/>
       <c r="AN18" s="12"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
@@ -24907,7 +24907,7 @@
       <c r="AM19" s="14"/>
       <c r="AN19" s="15"/>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A22" s="31" t="s">
         <v>70</v>
       </c>
@@ -24922,7 +24922,7 @@
       <c r="J22" s="31"/>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A23" s="28" t="s">
         <v>1</v>
       </c>
@@ -24967,7 +24967,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>3</v>
       </c>
@@ -25012,7 +25012,7 @@
         <v>-597.80079573463001</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>56</v>
       </c>
@@ -25057,7 +25057,7 @@
         <v>-474.77478093796299</v>
       </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A26" s="18" t="s">
         <v>57</v>
       </c>
@@ -25102,7 +25102,7 @@
         <v>-123.026014796667</v>
       </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -25147,7 +25147,7 @@
         <v>-82.704318361679299</v>
       </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -25204,12 +25204,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>62</v>
       </c>
@@ -25221,7 +25221,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -25233,7 +25233,7 @@
       </c>
       <c r="AN2" s="3"/>
     </row>
-    <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -25355,7 +25355,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -25477,7 +25477,7 @@
         <v>-600.92598787117299</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -25599,7 +25599,7 @@
         <v>-477.89997307450602</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -25721,7 +25721,7 @@
         <v>-123.026014796667</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI7" s="73"/>
       <c r="AJ7" s="30"/>
       <c r="AK7" s="30"/>
@@ -25729,7 +25729,7 @@
       <c r="AM7" s="30"/>
       <c r="AN7" s="74"/>
     </row>
-    <row r="8" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -25851,7 +25851,7 @@
         <v>-84.300386392345203</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI9" s="73"/>
       <c r="AJ9" s="30"/>
       <c r="AK9" s="30"/>
@@ -25859,7 +25859,7 @@
       <c r="AM9" s="30"/>
       <c r="AN9" s="74"/>
     </row>
-    <row r="10" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>58</v>
       </c>
@@ -25981,7 +25981,7 @@
         <v>-685.22637426351821</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI11" s="11"/>
       <c r="AJ11" s="2"/>
       <c r="AK11" s="2"/>
@@ -25989,7 +25989,7 @@
       <c r="AM11" s="2"/>
       <c r="AN11" s="12"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
       <c r="AI12" s="11"/>
       <c r="AJ12" s="2"/>
       <c r="AK12" s="2"/>
@@ -26008,12 +26008,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="29" max="29" width="9.140625" customWidth="1"/>
+    <col min="29" max="29" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -26021,7 +26021,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>136</v>
       </c>
@@ -26056,7 +26056,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="F3" t="s">
         <v>144</v>
       </c>
@@ -26081,7 +26081,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2022</v>
       </c>
@@ -26168,7 +26168,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>146</v>
       </c>
@@ -26240,7 +26240,7 @@
       </c>
       <c r="AA5" s="94"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2025</v>
       </c>
@@ -26348,7 +26348,7 @@
         <v>2025</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2035</v>
       </c>
@@ -26456,7 +26456,7 @@
         <v>2035</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2045</v>
       </c>
@@ -26564,7 +26564,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2055</v>
       </c>
@@ -26672,7 +26672,7 @@
         <v>2055</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2065</v>
       </c>
@@ -26780,7 +26780,7 @@
         <v>2065</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2075</v>
       </c>
@@ -26888,7 +26888,7 @@
         <v>2075</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2085</v>
       </c>
@@ -26996,7 +26996,7 @@
         <v>2085</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2095</v>
       </c>
@@ -27104,7 +27104,7 @@
         <v>2095</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2105</v>
       </c>
@@ -27212,7 +27212,7 @@
         <v>2105</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2115</v>
       </c>
@@ -27320,7 +27320,7 @@
         <v>2115</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2125</v>
       </c>
@@ -27428,7 +27428,7 @@
         <v>2125</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2135</v>
       </c>
@@ -27536,7 +27536,7 @@
         <v>2135</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2145</v>
       </c>
@@ -27644,7 +27644,7 @@
         <v>2145</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2155</v>
       </c>
@@ -27752,21 +27752,21 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="E20" s="93"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="E21" s="93"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="E22" s="93"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="Y23">
         <v>2024</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="Y25" s="92">
         <f>Y6</f>
         <v>774.18650000000002</v>
@@ -27793,7 +27793,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="Y26" s="92">
         <f t="shared" ref="Y26:Y28" si="0">Y7</f>
         <v>786.11766999999804</v>
@@ -27832,7 +27832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="Y27" s="92">
         <f t="shared" si="0"/>
         <v>547.73282000000233</v>
@@ -27846,7 +27846,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="Y28" s="92">
         <f t="shared" si="0"/>
         <v>1036.925469999996</v>
@@ -27858,17 +27858,17 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="AH29" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="25:34" x14ac:dyDescent="0.3">
       <c r="Y33" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AB34" t="s">
         <v>155</v>
       </c>
@@ -27889,7 +27889,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA35">
         <v>2025</v>
       </c>
@@ -27912,7 +27912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA36">
         <v>2030</v>
       </c>
@@ -27935,7 +27935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA37">
         <v>2035</v>
       </c>
@@ -27958,7 +27958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA38">
         <v>2040</v>
       </c>
@@ -27979,7 +27979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA39">
         <v>2045</v>
       </c>
@@ -28000,7 +28000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="25:34" x14ac:dyDescent="0.3">
       <c r="Y40" s="80"/>
       <c r="AA40">
         <v>2050</v>
@@ -28022,12 +28022,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="25:34" x14ac:dyDescent="0.3">
       <c r="Y42" s="21" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AB43" s="21" t="s">
         <v>159</v>
       </c>
@@ -28039,7 +28039,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="44" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA44">
         <v>2025</v>
       </c>
@@ -28050,7 +28050,7 @@
       <c r="AC44" s="29"/>
       <c r="AD44" s="29"/>
     </row>
-    <row r="45" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="45" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA45">
         <v>2030</v>
       </c>
@@ -28061,7 +28061,7 @@
       <c r="AC45" s="29"/>
       <c r="AD45" s="29"/>
     </row>
-    <row r="46" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="46" spans="25:34" x14ac:dyDescent="0.3">
       <c r="Y46" t="s">
         <v>161</v>
       </c>
@@ -28075,7 +28075,7 @@
       <c r="AC46" s="29"/>
       <c r="AD46" s="29"/>
     </row>
-    <row r="47" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="47" spans="25:34" x14ac:dyDescent="0.3">
       <c r="Y47" s="29">
         <f>'Forest CO2 compiled 82924'!F18</f>
         <v>-887.39999999999986</v>
@@ -28088,7 +28088,7 @@
         <v>-764.4533486608201</v>
       </c>
     </row>
-    <row r="48" spans="25:34" x14ac:dyDescent="0.25">
+    <row r="48" spans="25:34" x14ac:dyDescent="0.3">
       <c r="AA48">
         <v>2045</v>
       </c>
@@ -28097,7 +28097,7 @@
         <v>-627.83076748044823</v>
       </c>
     </row>
-    <row r="49" spans="25:32" x14ac:dyDescent="0.25">
+    <row r="49" spans="25:32" x14ac:dyDescent="0.3">
       <c r="AA49">
         <v>2050</v>
       </c>
@@ -28106,7 +28106,7 @@
         <v>-908.19574259303045</v>
       </c>
     </row>
-    <row r="52" spans="25:32" x14ac:dyDescent="0.25">
+    <row r="52" spans="25:32" x14ac:dyDescent="0.3">
       <c r="AA52">
         <v>2025</v>
       </c>
@@ -28126,7 +28126,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="53" spans="25:32" x14ac:dyDescent="0.25">
+    <row r="53" spans="25:32" x14ac:dyDescent="0.3">
       <c r="Y53" t="s">
         <v>163</v>
       </c>
@@ -28161,16 +28161,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
     <col min="4" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="26" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="26" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>107</v>
       </c>
@@ -28208,7 +28208,7 @@
       <c r="BE1" s="98"/>
       <c r="BF1" s="99"/>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>108</v>
       </c>
@@ -28381,11 +28381,11 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AE3" s="83"/>
       <c r="BF3" s="84"/>
     </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>129</v>
       </c>
@@ -28552,7 +28552,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:58" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="81" t="s">
         <v>125</v>
       </c>
@@ -28728,7 +28728,7 @@
         <v>189.73114988985805</v>
       </c>
     </row>
-    <row r="6" spans="1:58" s="102" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58" s="102" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="101" t="s">
         <v>130</v>
       </c>
@@ -28904,7 +28904,7 @@
         <v>56.405531914859935</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>125</v>
       </c>
@@ -29080,7 +29080,7 @@
         <v>16.221139354597913</v>
       </c>
     </row>
-    <row r="8" spans="1:58" s="105" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58" s="105" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="105" t="s">
         <v>127</v>
       </c>
@@ -29256,7 +29256,7 @@
         <v>286.00410299257976</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" s="82" t="s">
         <v>128</v>
       </c>
@@ -29432,18 +29432,18 @@
         <v>9.0411637688899198</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AE10" s="83"/>
       <c r="BF10" s="84"/>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>119</v>
       </c>
       <c r="AE11" s="83"/>
       <c r="BF11" s="84"/>
     </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -29619,7 +29619,7 @@
         <v>5.3274180301779497</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -29795,7 +29795,7 @@
         <v>3.2680026973139538</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -29971,7 +29971,7 @@
         <v>0.62064259018248991</v>
       </c>
     </row>
-    <row r="15" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>126</v>
       </c>
@@ -30147,11 +30147,11 @@
         <v>0.20234419203804235</v>
       </c>
     </row>
-    <row r="16" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="AE16" s="83"/>
       <c r="BF16" s="84"/>
     </row>
-    <row r="17" spans="1:58" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:58" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" t="s">
         <v>124</v>
       </c>
@@ -30275,7 +30275,7 @@
       <c r="BE17" s="90"/>
       <c r="BF17" s="91"/>
     </row>
-    <row r="18" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>131</v>
       </c>
@@ -30384,12 +30384,12 @@
         <v>566.82149543049786</v>
       </c>
     </row>
-    <row r="19" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C19" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>189</v>
       </c>
@@ -30606,13 +30606,13 @@
         <v>255.79848816379038</v>
       </c>
     </row>
-    <row r="21" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="J21" s="83"/>
     </row>
-    <row r="22" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C22" s="2" t="s">
         <v>190</v>
       </c>
@@ -30829,7 +30829,7 @@
         <v>302.42758653921572</v>
       </c>
     </row>
-    <row r="23" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -30844,7 +30844,7 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
     </row>
-    <row r="24" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C24" s="139" t="s">
         <v>191</v>
       </c>
@@ -31063,7 +31063,7 @@
         <v>8.5954207274919039</v>
       </c>
     </row>
-    <row r="25" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C25" s="102"/>
       <c r="D25" s="102"/>
       <c r="E25" s="102"/>
@@ -31080,13 +31080,13 @@
       <c r="P25" s="102"/>
       <c r="Q25" s="102"/>
     </row>
-    <row r="26" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:58" x14ac:dyDescent="0.3">
       <c r="G26" s="80"/>
       <c r="H26" s="80"/>
       <c r="I26" s="80"/>
       <c r="J26" s="88"/>
     </row>
-    <row r="27" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:58" x14ac:dyDescent="0.3">
       <c r="C27" s="105"/>
       <c r="D27" s="105"/>
       <c r="E27" s="105"/>
@@ -31103,40 +31103,40 @@
       <c r="P27" s="105"/>
       <c r="Q27" s="105"/>
     </row>
-    <row r="28" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:58" x14ac:dyDescent="0.3">
       <c r="G28" s="80"/>
       <c r="H28" s="80"/>
       <c r="I28" s="80"/>
       <c r="J28" s="88"/>
     </row>
-    <row r="29" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:58" x14ac:dyDescent="0.3">
       <c r="G29" s="80"/>
       <c r="H29" s="80"/>
       <c r="I29" s="80"/>
       <c r="J29" s="88"/>
     </row>
-    <row r="30" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:58" x14ac:dyDescent="0.3">
       <c r="G30" s="80"/>
       <c r="H30" s="80"/>
       <c r="I30" s="80"/>
       <c r="J30" s="88"/>
     </row>
-    <row r="31" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:58" x14ac:dyDescent="0.3">
       <c r="J31" s="83"/>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="J32" s="83"/>
     </row>
-    <row r="33" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J33" s="83"/>
     </row>
-    <row r="34" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J34" s="83"/>
     </row>
-    <row r="35" spans="10:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="10:17" x14ac:dyDescent="0.3">
       <c r="J35" s="83"/>
     </row>
-    <row r="36" spans="10:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="10:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J36" s="89"/>
       <c r="K36" s="90"/>
       <c r="L36" s="90"/>
@@ -31156,20 +31156,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B4A0C6-FB3D-48AD-8074-AF9061A88699}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>224</v>
       </c>
@@ -31204,7 +31204,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>213</v>
       </c>
@@ -31245,7 +31245,7 @@
         <v>-719.72637426351821</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>232</v>
       </c>
@@ -31286,7 +31286,7 @@
         <v>58.594755542095413</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>232</v>
       </c>
@@ -31327,7 +31327,7 @@
         <v>9.4825687076057825</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>214</v>
       </c>
@@ -31375,19 +31375,19 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.28515625" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="70.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="9.109375" customWidth="1"/>
     <col min="38" max="38" width="5" customWidth="1"/>
-    <col min="39" max="42" width="9.140625" customWidth="1"/>
+    <col min="39" max="42" width="9.109375" customWidth="1"/>
     <col min="43" max="43" width="5" customWidth="1"/>
-    <col min="44" max="64" width="9.140625" customWidth="1"/>
+    <col min="44" max="64" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -31581,7 +31581,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:64" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:64" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>223</v>
       </c>
@@ -31691,7 +31691,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="3" spans="1:64" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:64" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>223</v>
       </c>
@@ -31801,7 +31801,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="4" spans="1:64" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:64" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>223</v>
       </c>
@@ -31911,7 +31911,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -32021,7 +32021,7 @@
         <v>-787</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -32131,7 +32131,7 @@
         <v>-100.3</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -32241,7 +32241,7 @@
         <v>-787</v>
       </c>
     </row>
-    <row r="8" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -32351,7 +32351,7 @@
         <v>-100.3</v>
       </c>
     </row>
-    <row r="9" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -32461,7 +32461,7 @@
         <v>-787</v>
       </c>
     </row>
-    <row r="10" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -32571,7 +32571,7 @@
         <v>-100.3</v>
       </c>
     </row>
-    <row r="11" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -32681,7 +32681,7 @@
         <v>-31.7</v>
       </c>
     </row>
-    <row r="12" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -32791,7 +32791,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="13" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -32901,7 +32901,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="14" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -33011,7 +33011,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="15" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -33121,7 +33121,7 @@
         <v>-10.6</v>
       </c>
     </row>
-    <row r="16" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -33231,7 +33231,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -33341,7 +33341,7 @@
         <v>-134.80000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -33451,7 +33451,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="19" spans="1:64" s="157" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:64" s="157" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="157" t="s">
         <v>13</v>
       </c>
@@ -33588,7 +33588,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -33782,7 +33782,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -33976,7 +33976,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -34086,7 +34086,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
@@ -34196,7 +34196,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -34306,7 +34306,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -34416,7 +34416,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
@@ -34526,7 +34526,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>18</v>
       </c>
@@ -34636,7 +34636,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="28" spans="1:64" s="156" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" s="156" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="156" t="s">
         <v>19</v>
       </c>
@@ -34773,7 +34773,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -34967,7 +34967,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="30" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -35161,7 +35161,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="31" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>26</v>
       </c>
@@ -35355,7 +35355,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -35465,7 +35465,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -35575,7 +35575,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>16</v>
       </c>
@@ -35685,7 +35685,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>212</v>
       </c>
@@ -35795,7 +35795,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="36" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="21" t="s">
         <v>211</v>
       </c>
@@ -35905,7 +35905,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="37" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="21" t="s">
         <v>211</v>
       </c>
@@ -36015,7 +36015,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="38" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:36" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="21" t="s">
         <v>211</v>
       </c>
@@ -36125,7 +36125,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="39" spans="1:36" s="159" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:36" s="159" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="159" t="s">
         <v>210</v>
       </c>
@@ -36235,7 +36235,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="40" spans="1:36" s="158" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:36" s="158" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="158" t="s">
         <v>209</v>
       </c>
@@ -36345,7 +36345,7 @@
         <v>-854.3</v>
       </c>
     </row>
-    <row r="41" spans="1:36" s="158" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:36" s="158" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="158" t="s">
         <v>209</v>
       </c>
@@ -36455,7 +36455,7 @@
         <v>-854.3</v>
       </c>
     </row>
-    <row r="42" spans="1:36" s="158" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:36" s="158" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="158" t="s">
         <v>209</v>
       </c>
@@ -36581,15 +36581,15 @@
       <selection activeCell="G10" sqref="G10:L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="34" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>202</v>
       </c>
@@ -36597,7 +36597,7 @@
         <v>45533</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="31" t="s">
         <v>205</v>
       </c>
@@ -36612,7 +36612,7 @@
         <v>PROJECTIONS</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="30" t="str">
         <f>'USFS Forest CO2 73024_OLD'!A23</f>
         <v>Gas/Land-Use Category</v>
@@ -36658,7 +36658,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="51" t="str">
         <f>'USFS Forest CO2 73024_OLD'!A24</f>
         <v>Forest Land Remaining Forest Land</v>
@@ -36704,7 +36704,7 @@
         <v>-600.92598787117299</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="52" t="str">
         <f>'USFS Forest CO2 73024_OLD'!A25</f>
         <v>Changes in Forest Carbon Stocks</v>
@@ -36750,7 +36750,7 @@
         <v>-477.89997307450602</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="52" t="str">
         <f>'USFS Forest CO2 73024_OLD'!A26</f>
         <v>HWP and SWD</v>
@@ -36796,7 +36796,7 @@
         <v>-123.026014796667</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="52" t="str">
         <f>'USFS Forest CO2 73024_OLD'!A27</f>
         <v>Land Converted to Forest Land</v>
@@ -36842,7 +36842,7 @@
         <v>-84.300386392345203</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>207</v>
       </c>
@@ -36890,8 +36890,8 @@
         <v>-685.22637426351821</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="109" t="s">
         <v>71</v>
       </c>
@@ -36936,7 +36936,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
       <c r="B14" s="109" t="s">
         <v>72</v>
@@ -36982,13 +36982,13 @@
         <v>-719.72637426351821</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="116" t="s">
         <v>206</v>
       </c>
       <c r="B16" s="116"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17" s="61"/>
       <c r="B17" s="62"/>
       <c r="C17" s="115">
@@ -37024,7 +37024,7 @@
       </c>
       <c r="M17" s="120"/>
     </row>
-    <row r="18" spans="1:16" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="147" t="s">
         <v>207</v>
       </c>
@@ -37073,13 +37073,13 @@
       </c>
       <c r="M18" s="119"/>
     </row>
-    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C19" s="29"/>
       <c r="D19" s="29"/>
       <c r="E19" s="29"/>
       <c r="F19" s="29"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="109" t="str">
         <f>B13</f>
         <v xml:space="preserve">ALL LULUCFCO2 using </v>
@@ -37116,7 +37116,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="109"/>
       <c r="B21" s="109" t="s">
         <v>164</v>
@@ -37162,8 +37162,8 @@
         <v>-942.59339914671614</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>153</v>
       </c>
@@ -37196,7 +37196,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>152</v>
       </c>
@@ -37238,7 +37238,7 @@
         <v>-719.72637426351821</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>151</v>
       </c>
@@ -37281,12 +37281,12 @@
       </c>
       <c r="M27" s="29"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="25" t="s">
         <v>204</v>
       </c>
@@ -37308,7 +37308,7 @@
       <c r="O30" s="22"/>
       <c r="P30" s="22"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" s="46"/>
       <c r="C31" s="37" t="s">
         <v>65</v>
@@ -37325,7 +37325,7 @@
       <c r="K31" s="38"/>
       <c r="L31" s="39"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32" s="47"/>
       <c r="C32" s="40">
         <f>'nonforestCO2 GHGI 81224'!C4</f>
@@ -37367,7 +37367,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B33" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B5</f>
         <v>Cropland Remaining Cropland</v>
@@ -37413,7 +37413,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B34" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B6</f>
         <v>Land Converted to Cropland</v>
@@ -37459,7 +37459,7 @@
         <v>33.814367644374251</v>
       </c>
     </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B35" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B7</f>
         <v>Grassland Remaining Grassland</v>
@@ -37505,7 +37505,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B36" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B8</f>
         <v>Land Converted to Grassland</v>
@@ -37551,7 +37551,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B37" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B9</f>
         <v>Wetlands Remaining Wetlands</v>
@@ -37597,7 +37597,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B38" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B10</f>
         <v>Land Converted to Wetlands</v>
@@ -37643,7 +37643,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B39" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B11</f>
         <v>Settlements Remaining Settlements*</v>
@@ -37689,7 +37689,7 @@
         <v>-171.73140746240804</v>
       </c>
     </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B40" s="47" t="str">
         <f>'nonforestCO2 GHGI 81224'!B12</f>
         <v>Land Converted to Settlements</v>
@@ -37735,7 +37735,7 @@
         <v>86.820474343485756</v>
       </c>
     </row>
-    <row r="41" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="48" t="str">
         <f>'nonforestCO2 GHGI 81224'!B13</f>
         <v>subtotal non-forest LUC CO2</v>
@@ -37801,13 +37801,13 @@
       <selection pane="bottomRight" activeCell="AJ47" sqref="AJ47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="54" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>107</v>
       </c>
@@ -37818,12 +37818,12 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:63" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:63" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="79" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>79</v>
       </c>
@@ -38014,7 +38014,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -38205,7 +38205,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>82</v>
       </c>
@@ -38396,7 +38396,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="6" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -38587,7 +38587,7 @@
         <v>33.814367644374251</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -38778,7 +38778,7 @@
         <v>33.814367644374251</v>
       </c>
     </row>
-    <row r="8" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -38969,7 +38969,7 @@
         <v>5.064333299052576</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -39160,7 +39160,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="10" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -39351,7 +39351,7 @@
         <v>0.59462816708368171</v>
       </c>
     </row>
-    <row r="11" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
@@ -39542,7 +39542,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="12" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>84</v>
       </c>
@@ -39733,7 +39733,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -39924,7 +39924,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="14" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>89</v>
       </c>
@@ -40115,7 +40115,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="15" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>90</v>
       </c>
@@ -40306,7 +40306,7 @@
         <v>1.2737501172567186E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>91</v>
       </c>
@@ -40497,7 +40497,7 @@
         <v>-11.1</v>
       </c>
     </row>
-    <row r="17" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>92</v>
       </c>
@@ -40688,7 +40688,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="18" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>93</v>
       </c>
@@ -40879,7 +40879,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>94</v>
       </c>
@@ -41070,7 +41070,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="20" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -41261,7 +41261,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="21" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -41452,7 +41452,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -41643,7 +41643,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -41834,7 +41834,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="24" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -42025,7 +42025,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -42216,7 +42216,7 @@
         <v>-168.54883875480226</v>
       </c>
     </row>
-    <row r="26" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>102</v>
       </c>
@@ -42407,7 +42407,7 @@
         <v>19.604623238851623</v>
       </c>
     </row>
-    <row r="27" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>103</v>
       </c>
@@ -42598,7 +42598,7 @@
         <v>-176.31430640136037</v>
       </c>
     </row>
-    <row r="28" spans="1:63" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:63" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -42789,7 +42789,7 @@
         <v>3.1825687076057827</v>
       </c>
     </row>
-    <row r="29" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>105</v>
       </c>
@@ -42980,7 +42980,7 @@
         <v>-15.021724299899295</v>
       </c>
     </row>
-    <row r="30" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>12</v>
       </c>
@@ -43171,7 +43171,7 @@
         <v>86.820474343485756</v>
       </c>
     </row>
-    <row r="31" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>84</v>
       </c>
@@ -43362,7 +43362,7 @@
         <v>86.820474343485756</v>
       </c>
     </row>
-    <row r="32" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:63" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>199</v>
       </c>
@@ -43611,12 +43611,12 @@
         <v>-82.138390239101824</v>
       </c>
     </row>
-    <row r="34" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A34" s="152" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="35" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -43865,7 +43865,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="36" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A36" s="80" t="str">
         <f>A4</f>
         <v>Cropland Remaining Cropland</v>
@@ -43874,7 +43874,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="37" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A37" s="80" t="str">
         <f>A6</f>
         <v>Land Converted to Cropland</v>
@@ -43883,7 +43883,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="38" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A38" s="80" t="str">
         <f>A8</f>
         <v>Grassland Remaining Grassland</v>
@@ -44133,7 +44133,7 @@
         <v>0.59462816708368171</v>
       </c>
     </row>
-    <row r="39" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A39" s="80" t="str">
         <f>A11</f>
         <v>Land Converted to Grassland</v>
@@ -44142,7 +44142,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:63" s="80" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="80" t="str">
         <f>A13</f>
         <v>Wetlands Remaining Wetlands</v>
@@ -44392,7 +44392,7 @@
         <v>48.500127375011729</v>
       </c>
     </row>
-    <row r="41" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A41" s="80" t="str">
         <f>A20</f>
         <v>Land Converted to Wetlands</v>
@@ -44642,7 +44642,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A42" s="80" t="str">
         <f>A25</f>
         <v>Settlements Remaining Settlements</v>
@@ -44651,7 +44651,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A43" s="80" t="str">
         <f>A30</f>
         <v>Land Converted to Settlements</v>
@@ -44660,13 +44660,13 @@
         <v>195</v>
       </c>
     </row>
-    <row r="44" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A44" s="80"/>
       <c r="B44" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="45" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:63" x14ac:dyDescent="0.3">
       <c r="C45" s="2">
         <f>SUM(C36:C43)</f>
         <v>49.90023985513772</v>
@@ -44912,7 +44912,7 @@
         <v>49.494755542095412</v>
       </c>
     </row>
-    <row r="46" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:63" x14ac:dyDescent="0.3">
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
@@ -44975,7 +44975,7 @@
       <c r="BJ46" s="2"/>
       <c r="BK46" s="2"/>
     </row>
-    <row r="47" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>19</v>
       </c>
@@ -45163,7 +45163,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="48" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -45171,7 +45171,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="49" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>6</v>
       </c>
@@ -45179,7 +45179,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="50" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -45193,7 +45193,7 @@
       <c r="AP50" s="92"/>
       <c r="AQ50" s="92"/>
     </row>
-    <row r="51" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>8</v>
       </c>
@@ -45201,7 +45201,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="52" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>9</v>
       </c>
@@ -45450,7 +45450,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="53" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>10</v>
       </c>
@@ -45458,7 +45458,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="54" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>11</v>
       </c>
@@ -45707,7 +45707,7 @@
         <v>3.1825687076057827</v>
       </c>
     </row>
-    <row r="55" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>12</v>
       </c>
@@ -45715,15 +45715,15 @@
         <v>195</v>
       </c>
     </row>
-    <row r="56" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AK56" s="2"/>
     </row>
-    <row r="57" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="58" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C58" s="2">
         <f>SUM(C48:C55)</f>
         <v>2.2000000000000002</v>
@@ -45969,7 +45969,7 @@
         <v>3.2825687076057828</v>
       </c>
     </row>
-    <row r="61" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AJ61" s="2" t="s">
         <v>121</v>
       </c>
@@ -45977,7 +45977,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>121</v>
       </c>
@@ -46165,7 +46165,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="63" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -46414,7 +46414,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="64" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>6</v>
       </c>
@@ -46663,7 +46663,7 @@
         <v>33.814367644374251</v>
       </c>
     </row>
-    <row r="65" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>7</v>
       </c>
@@ -46912,7 +46912,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="66" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>8</v>
       </c>
@@ -47161,7 +47161,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="67" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A67" s="80" t="s">
         <v>9</v>
       </c>
@@ -47410,7 +47410,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="68" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>10</v>
       </c>
@@ -47659,7 +47659,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="69" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>11</v>
       </c>
@@ -47908,7 +47908,7 @@
         <v>-171.73140746240804</v>
       </c>
     </row>
-    <row r="70" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>12</v>
       </c>
@@ -48157,12 +48157,12 @@
         <v>86.820474343485756</v>
       </c>
     </row>
-    <row r="71" spans="1:63" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:63" ht="14.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B71" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="72" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:63" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="C72" s="2">
         <f>SUM(C63:C70)</f>
         <v>40.499999999999993</v>
@@ -48408,7 +48408,7 @@
         <v>-82.138390239101824</v>
       </c>
     </row>
-    <row r="77" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AI77" s="2" t="s">
         <v>121</v>
       </c>
@@ -48431,7 +48431,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="78" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AI78" t="s">
         <v>5</v>
       </c>
@@ -48460,7 +48460,7 @@
         <v>-50.533150996586201</v>
       </c>
     </row>
-    <row r="79" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AI79" t="s">
         <v>6</v>
       </c>
@@ -48489,7 +48489,7 @@
         <v>33.814367644374251</v>
       </c>
     </row>
-    <row r="80" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:63" x14ac:dyDescent="0.3">
       <c r="AI80" t="s">
         <v>7</v>
       </c>
@@ -48518,7 +48518,7 @@
         <v>4.4697051319688939</v>
       </c>
     </row>
-    <row r="81" spans="35:43" x14ac:dyDescent="0.25">
+    <row r="81" spans="35:43" x14ac:dyDescent="0.3">
       <c r="AI81" t="s">
         <v>8</v>
       </c>
@@ -48547,7 +48547,7 @@
         <v>25.221621100063519</v>
       </c>
     </row>
-    <row r="82" spans="35:43" x14ac:dyDescent="0.25">
+    <row r="82" spans="35:43" x14ac:dyDescent="0.3">
       <c r="AI82" s="80" t="s">
         <v>9</v>
       </c>
@@ -48576,7 +48576,7 @@
         <v>-10.5</v>
       </c>
     </row>
-    <row r="83" spans="35:43" x14ac:dyDescent="0.25">
+    <row r="83" spans="35:43" x14ac:dyDescent="0.3">
       <c r="AI83" t="s">
         <v>10</v>
       </c>
@@ -48605,7 +48605,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="84" spans="35:43" x14ac:dyDescent="0.25">
+    <row r="84" spans="35:43" x14ac:dyDescent="0.3">
       <c r="AI84" t="s">
         <v>11</v>
       </c>
@@ -48634,7 +48634,7 @@
         <v>-171.73140746240804</v>
       </c>
     </row>
-    <row r="85" spans="35:43" x14ac:dyDescent="0.25">
+    <row r="85" spans="35:43" x14ac:dyDescent="0.3">
       <c r="AI85" t="s">
         <v>12</v>
       </c>
@@ -48677,14 +48677,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="1" max="1" width="53.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>73</v>
       </c>
@@ -48692,8 +48692,8 @@
         <v>45533</v>
       </c>
     </row>
-    <row r="2" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:60" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:60" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>75</v>
       </c>
@@ -48708,7 +48708,7 @@
       </c>
       <c r="AN3" s="64"/>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>193</v>
       </c>
@@ -48890,7 +48890,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -49072,7 +49072,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -49254,7 +49254,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -49436,7 +49436,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -49618,7 +49618,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -49800,7 +49800,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -49982,7 +49982,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:60" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -50164,7 +50164,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:60" x14ac:dyDescent="0.3">
       <c r="AI12" s="42"/>
       <c r="AJ12" s="36"/>
       <c r="AK12" s="36"/>
@@ -50192,7 +50192,7 @@
       <c r="BG12" s="43"/>
       <c r="BH12" s="43"/>
     </row>
-    <row r="13" spans="1:60" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:60" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>194</v>
       </c>
@@ -50449,14 +50449,14 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.5703125" style="166" bestFit="1" customWidth="1"/>
-    <col min="2" max="27" width="5.5703125" style="166" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="166"/>
+    <col min="1" max="1" width="53.5546875" style="166" bestFit="1" customWidth="1"/>
+    <col min="2" max="27" width="5.5546875" style="166" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.109375" style="166"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="166" t="s">
         <v>193</v>
       </c>
@@ -50539,7 +50539,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="165" t="s">
         <v>13</v>
       </c>
@@ -50570,7 +50570,7 @@
       <c r="Z2" s="165"/>
       <c r="AA2" s="165"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="166" t="s">
         <v>25</v>
       </c>
@@ -50653,7 +50653,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="166" t="s">
         <v>26</v>
       </c>
@@ -50736,7 +50736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="165" t="s">
         <v>19</v>
       </c>
@@ -50767,7 +50767,7 @@
       <c r="Z5" s="165"/>
       <c r="AA5" s="165"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="166" t="s">
         <v>25</v>
       </c>
@@ -50850,7 +50850,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="166" t="s">
         <v>29</v>
       </c>
@@ -50933,7 +50933,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="166" t="s">
         <v>26</v>
       </c>
@@ -51016,7 +51016,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="166" t="s">
         <v>194</v>
       </c>
@@ -51125,12 +51125,12 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="166" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="166" t="s">
         <v>13</v>
       </c>
@@ -51213,17 +51213,17 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="166" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="166" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="166" t="s">
         <v>7</v>
       </c>
@@ -51306,12 +51306,12 @@
         <v>0.59462816708368171</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="166" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="166" t="s">
         <v>9</v>
       </c>
@@ -51394,7 +51394,7 @@
         <v>48.500127375011729</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="166" t="s">
         <v>10</v>
       </c>
@@ -51477,17 +51477,17 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="166" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="166" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="166" t="s">
         <v>196</v>
       </c>
@@ -51570,7 +51570,7 @@
         <v>49.494755542095412</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" s="166" t="s">
         <v>19</v>
       </c>
@@ -51653,27 +51653,27 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" s="166" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" s="166" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29" s="166" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30" s="166" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31" s="166" t="s">
         <v>9</v>
       </c>
@@ -51756,12 +51756,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" s="166" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" s="166" t="s">
         <v>11</v>
       </c>
@@ -51844,12 +51844,12 @@
         <v>3.1825687076057827</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" s="166" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" s="166" t="s">
         <v>197</v>
       </c>
@@ -51932,7 +51932,7 @@
         <v>3.2825687076057828</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" s="166" t="s">
         <v>234</v>
       </c>
@@ -52041,7 +52041,7 @@
         <v>58.594755542095413</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" s="166" t="s">
         <v>235</v>
       </c>
@@ -52159,19 +52159,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH43"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="70.28515625" customWidth="1"/>
+    <col min="1" max="1" width="70.33203125" customWidth="1"/>
+    <col min="18" max="21" width="8.88671875" customWidth="1"/>
+    <col min="23" max="26" width="8.88671875" customWidth="1"/>
+    <col min="28" max="31" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" s="154" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -52275,7 +52280,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -52379,7 +52384,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -52483,7 +52488,7 @@
         <v>-787</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -52587,7 +52592,7 @@
         <v>-100.3</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -52691,7 +52696,7 @@
         <v>-31.7</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -52795,7 +52800,7 @@
         <v>35.1</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -52899,7 +52904,7 @@
         <v>13.4</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -53003,7 +53008,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -53107,7 +53112,7 @@
         <v>-10.6</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -53211,7 +53216,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -53315,7 +53320,7 @@
         <v>-134.80000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -53419,7 +53424,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -53523,7 +53528,7 @@
         <v>58.4</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -53627,7 +53632,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -53731,7 +53736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -53835,7 +53840,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -53939,7 +53944,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -54043,7 +54048,7 @@
         <v>4.3</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -54147,7 +54152,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -54251,7 +54256,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -54355,7 +54360,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -54459,7 +54464,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -54563,7 +54568,7 @@
         <v>5.7</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -54667,7 +54672,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -54771,7 +54776,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -54875,7 +54880,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -54979,7 +54984,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -55083,7 +55088,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -55187,7 +55192,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -55291,7 +55296,7 @@
         <v>-921.8</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>21</v>
       </c>
@@ -55395,7 +55400,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -55499,52 +55504,52 @@
         <v>-854.3</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -55560,17 +55565,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="34" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="34" width="6.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -55674,7 +55679,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -55778,7 +55783,7 @@
         <v>-694.3</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -55882,7 +55887,7 @@
         <v>-491.7</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -55986,7 +55991,7 @@
         <v>-96.9</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -56090,7 +56095,7 @@
         <v>-131.4</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>45</v>
       </c>
@@ -56194,7 +56199,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -56298,7 +56303,7 @@
         <v>-1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>47</v>
       </c>
@@ -56402,7 +56407,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>48</v>
       </c>
@@ -56506,7 +56511,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -56610,7 +56615,7 @@
         <v>-92.8</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -56714,7 +56719,7 @@
         <v>-28.8</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>51</v>
       </c>
@@ -56818,7 +56823,7 @@
         <v>-63.9</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -56922,12 +56927,12 @@
         <v>-787</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>54</v>
       </c>

</xml_diff>